<commit_message>
more edits (eg added additional cols to baseline tsvs that was in time point csv)
</commit_message>
<xml_diff>
--- a/data_dictionaries/jcoin_core_measure_data_dictionaries.xlsx
+++ b/data_dictionaries/jcoin_core_measure_data_dictionaries.xlsx
@@ -3642,7 +3642,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M186"/>
+  <dimension ref="A1:M241"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12849,6 +12849,2737 @@
         </is>
       </c>
     </row>
+    <row r="187">
+      <c r="A187" s="1" t="n">
+        <v>185</v>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>PROMIS 29+2/ PROPr</t>
+        </is>
+      </c>
+      <c r="C187" t="inlineStr">
+        <is>
+          <t>p1a</t>
+        </is>
+      </c>
+      <c r="D187" t="inlineStr">
+        <is>
+          <t>p1</t>
+        </is>
+      </c>
+      <c r="E187" t="inlineStr">
+        <is>
+          <t>Difficulty with chores and house keeping</t>
+        </is>
+      </c>
+      <c r="F187" t="inlineStr"/>
+      <c r="G187" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="H187" t="inlineStr"/>
+      <c r="I187" t="inlineStr"/>
+      <c r="J187" t="inlineStr">
+        <is>
+          <t>['Without any difficulty', ' With a little difficulty', '  With some difficulty', ' With much difficulty', ' Unable to do']</t>
+        </is>
+      </c>
+      <c r="K187" t="inlineStr">
+        <is>
+          <t>In the past 7 days I was able to . . .</t>
+        </is>
+      </c>
+      <c r="L187" t="inlineStr">
+        <is>
+          <t>... do chores such as sweeping, mopping, janitorial work or other house cleaning work</t>
+        </is>
+      </c>
+      <c r="M187" t="inlineStr"/>
+    </row>
+    <row r="188">
+      <c r="A188" s="1" t="n">
+        <v>186</v>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>PROMIS 29+2/ PROPr</t>
+        </is>
+      </c>
+      <c r="C188" t="inlineStr">
+        <is>
+          <t>p1b</t>
+        </is>
+      </c>
+      <c r="D188" t="inlineStr">
+        <is>
+          <t>p1</t>
+        </is>
+      </c>
+      <c r="E188" t="inlineStr">
+        <is>
+          <t>Difficulty using stairs</t>
+        </is>
+      </c>
+      <c r="F188" t="inlineStr"/>
+      <c r="G188" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="H188" t="inlineStr"/>
+      <c r="I188" t="inlineStr"/>
+      <c r="J188" t="inlineStr">
+        <is>
+          <t>['Without any difficulty', ' With a little difficulty', '  With some difficulty', ' With much difficulty', ' Unable to do']</t>
+        </is>
+      </c>
+      <c r="K188" t="inlineStr">
+        <is>
+          <t>In the past 7 days I was able to . . .</t>
+        </is>
+      </c>
+      <c r="L188" t="inlineStr">
+        <is>
+          <t>...go up and down stairs at a normal pace</t>
+        </is>
+      </c>
+      <c r="M188" t="inlineStr"/>
+    </row>
+    <row r="189">
+      <c r="A189" s="1" t="n">
+        <v>187</v>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>PROMIS 29+2/ PROPr</t>
+        </is>
+      </c>
+      <c r="C189" t="inlineStr">
+        <is>
+          <t>p1c</t>
+        </is>
+      </c>
+      <c r="D189" t="inlineStr">
+        <is>
+          <t>p1</t>
+        </is>
+      </c>
+      <c r="E189" t="inlineStr">
+        <is>
+          <t>Difficulty walking</t>
+        </is>
+      </c>
+      <c r="F189" t="inlineStr"/>
+      <c r="G189" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="H189" t="inlineStr"/>
+      <c r="I189" t="inlineStr"/>
+      <c r="J189" t="inlineStr">
+        <is>
+          <t>['Without any difficulty', ' With a little difficulty', '  With some difficulty', ' With much difficulty', ' Unable to do']</t>
+        </is>
+      </c>
+      <c r="K189" t="inlineStr">
+        <is>
+          <t>In the past 7 days I was able to . . .</t>
+        </is>
+      </c>
+      <c r="L189" t="inlineStr">
+        <is>
+          <t>...walk around for at least 15 minutes</t>
+        </is>
+      </c>
+      <c r="M189" t="inlineStr"/>
+    </row>
+    <row r="190">
+      <c r="A190" s="1" t="n">
+        <v>188</v>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>PROMIS 29+2/ PROPr</t>
+        </is>
+      </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t>p1d</t>
+        </is>
+      </c>
+      <c r="D190" t="inlineStr">
+        <is>
+          <t>p1</t>
+        </is>
+      </c>
+      <c r="E190" t="inlineStr">
+        <is>
+          <t>Difficulty traveling</t>
+        </is>
+      </c>
+      <c r="F190" t="inlineStr"/>
+      <c r="G190" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="H190" t="inlineStr"/>
+      <c r="I190" t="inlineStr"/>
+      <c r="J190" t="inlineStr">
+        <is>
+          <t>['Without any difficulty', ' With a little difficulty', '  With some difficulty', ' With much difficulty', ' Unable to do']</t>
+        </is>
+      </c>
+      <c r="K190" t="inlineStr">
+        <is>
+          <t>In the past 7 days I was able to . . .</t>
+        </is>
+      </c>
+      <c r="L190" t="inlineStr">
+        <is>
+          <t>... get from place to place</t>
+        </is>
+      </c>
+      <c r="M190" t="inlineStr"/>
+    </row>
+    <row r="191">
+      <c r="A191" s="1" t="n">
+        <v>189</v>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>PROMIS 29+2/ PROPr</t>
+        </is>
+      </c>
+      <c r="C191" t="inlineStr">
+        <is>
+          <t>p2a</t>
+        </is>
+      </c>
+      <c r="D191" t="inlineStr">
+        <is>
+          <t>p2</t>
+        </is>
+      </c>
+      <c r="E191" t="inlineStr">
+        <is>
+          <t>Trouble with Leisure activities with others</t>
+        </is>
+      </c>
+      <c r="F191" t="inlineStr"/>
+      <c r="G191" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="H191" t="inlineStr"/>
+      <c r="I191" t="inlineStr"/>
+      <c r="J191" t="inlineStr">
+        <is>
+          <t>['Never', 'Rarely', 'Sometimes', 'Often', 'Always']</t>
+        </is>
+      </c>
+      <c r="K191" t="inlineStr">
+        <is>
+          <t>In the past 7 days…</t>
+        </is>
+      </c>
+      <c r="L191" t="inlineStr">
+        <is>
+          <t>...I had trouble doing all of my regular leisure activities with others</t>
+        </is>
+      </c>
+      <c r="M191" t="inlineStr"/>
+    </row>
+    <row r="192">
+      <c r="A192" s="1" t="n">
+        <v>190</v>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>PROMIS 29+2/ PROPr</t>
+        </is>
+      </c>
+      <c r="C192" t="inlineStr">
+        <is>
+          <t>p2b</t>
+        </is>
+      </c>
+      <c r="D192" t="inlineStr">
+        <is>
+          <t>p2</t>
+        </is>
+      </c>
+      <c r="E192" t="inlineStr">
+        <is>
+          <t>Trouble with family activities</t>
+        </is>
+      </c>
+      <c r="F192" t="inlineStr"/>
+      <c r="G192" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="H192" t="inlineStr"/>
+      <c r="I192" t="inlineStr"/>
+      <c r="J192" t="inlineStr">
+        <is>
+          <t>['Never', 'Rarely', 'Sometimes', 'Often', 'Always']</t>
+        </is>
+      </c>
+      <c r="K192" t="inlineStr">
+        <is>
+          <t>In the past 7 days…</t>
+        </is>
+      </c>
+      <c r="L192" t="inlineStr">
+        <is>
+          <t>...I had trouble doing all of the family activities that I want to do</t>
+        </is>
+      </c>
+      <c r="M192" t="inlineStr"/>
+    </row>
+    <row r="193">
+      <c r="A193" s="1" t="n">
+        <v>191</v>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>PROMIS 29+2/ PROPr</t>
+        </is>
+      </c>
+      <c r="C193" t="inlineStr">
+        <is>
+          <t>p2c</t>
+        </is>
+      </c>
+      <c r="D193" t="inlineStr">
+        <is>
+          <t>p2</t>
+        </is>
+      </c>
+      <c r="E193" t="inlineStr">
+        <is>
+          <t>Trouble with work</t>
+        </is>
+      </c>
+      <c r="F193" t="inlineStr"/>
+      <c r="G193" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="H193" t="inlineStr"/>
+      <c r="I193" t="inlineStr"/>
+      <c r="J193" t="inlineStr">
+        <is>
+          <t>['Never', 'Rarely', 'Sometimes', 'Often', 'Always']</t>
+        </is>
+      </c>
+      <c r="K193" t="inlineStr">
+        <is>
+          <t>In the past 7 days…</t>
+        </is>
+      </c>
+      <c r="L193" t="inlineStr">
+        <is>
+          <t>...I had trouble doing all of my usual work (include work at home)</t>
+        </is>
+      </c>
+      <c r="M193" t="inlineStr"/>
+    </row>
+    <row r="194">
+      <c r="A194" s="1" t="n">
+        <v>192</v>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>PROMIS 29+2/ PROPr</t>
+        </is>
+      </c>
+      <c r="C194" t="inlineStr">
+        <is>
+          <t>p2d</t>
+        </is>
+      </c>
+      <c r="D194" t="inlineStr">
+        <is>
+          <t>p2</t>
+        </is>
+      </c>
+      <c r="E194" t="inlineStr">
+        <is>
+          <t>Trouble with activities with friends</t>
+        </is>
+      </c>
+      <c r="F194" t="inlineStr"/>
+      <c r="G194" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="H194" t="inlineStr"/>
+      <c r="I194" t="inlineStr"/>
+      <c r="J194" t="inlineStr">
+        <is>
+          <t>['Never', 'Rarely', 'Sometimes', 'Often', 'Always']</t>
+        </is>
+      </c>
+      <c r="K194" t="inlineStr">
+        <is>
+          <t>In the past 7 days…</t>
+        </is>
+      </c>
+      <c r="L194" t="inlineStr">
+        <is>
+          <t>...I had trouble doing all of the activities with friends that I want to do</t>
+        </is>
+      </c>
+      <c r="M194" t="inlineStr"/>
+    </row>
+    <row r="195">
+      <c r="A195" s="1" t="n">
+        <v>193</v>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>PROMIS 29+2/ PROPr</t>
+        </is>
+      </c>
+      <c r="C195" t="inlineStr">
+        <is>
+          <t>p3a</t>
+        </is>
+      </c>
+      <c r="D195" t="inlineStr">
+        <is>
+          <t>p3</t>
+        </is>
+      </c>
+      <c r="E195" t="inlineStr">
+        <is>
+          <t>Feeling fearful</t>
+        </is>
+      </c>
+      <c r="F195" t="inlineStr"/>
+      <c r="G195" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="H195" t="inlineStr"/>
+      <c r="I195" t="inlineStr"/>
+      <c r="J195" t="inlineStr">
+        <is>
+          <t>['Never', 'Rarely', 'Sometimes', 'Often', 'Always']</t>
+        </is>
+      </c>
+      <c r="K195" t="inlineStr">
+        <is>
+          <t>In the past 7 days…</t>
+        </is>
+      </c>
+      <c r="L195" t="inlineStr">
+        <is>
+          <t>...I felt fearful</t>
+        </is>
+      </c>
+      <c r="M195" t="inlineStr"/>
+    </row>
+    <row r="196">
+      <c r="A196" s="1" t="n">
+        <v>194</v>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>PROMIS 29+2/ PROPr</t>
+        </is>
+      </c>
+      <c r="C196" t="inlineStr">
+        <is>
+          <t>p3b</t>
+        </is>
+      </c>
+      <c r="D196" t="inlineStr">
+        <is>
+          <t>p3</t>
+        </is>
+      </c>
+      <c r="E196" t="inlineStr">
+        <is>
+          <t>Feeling hard to focus on anything other than anxiety</t>
+        </is>
+      </c>
+      <c r="F196" t="inlineStr"/>
+      <c r="G196" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="H196" t="inlineStr"/>
+      <c r="I196" t="inlineStr"/>
+      <c r="J196" t="inlineStr">
+        <is>
+          <t>['Never', 'Rarely', 'Sometimes', 'Often', 'Always']</t>
+        </is>
+      </c>
+      <c r="K196" t="inlineStr">
+        <is>
+          <t>In the past 7 days…</t>
+        </is>
+      </c>
+      <c r="L196" t="inlineStr">
+        <is>
+          <t>...I found it hard to focus on anything other than my anxiety</t>
+        </is>
+      </c>
+      <c r="M196" t="inlineStr"/>
+    </row>
+    <row r="197">
+      <c r="A197" s="1" t="n">
+        <v>195</v>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>PROMIS 29+2/ PROPr</t>
+        </is>
+      </c>
+      <c r="C197" t="inlineStr">
+        <is>
+          <t>p3c</t>
+        </is>
+      </c>
+      <c r="D197" t="inlineStr">
+        <is>
+          <t>p3</t>
+        </is>
+      </c>
+      <c r="E197" t="inlineStr">
+        <is>
+          <t>Feeling overwhelming worry</t>
+        </is>
+      </c>
+      <c r="F197" t="inlineStr"/>
+      <c r="G197" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="H197" t="inlineStr"/>
+      <c r="I197" t="inlineStr"/>
+      <c r="J197" t="inlineStr">
+        <is>
+          <t>['Never', 'Rarely', 'Sometimes', 'Often', 'Always']</t>
+        </is>
+      </c>
+      <c r="K197" t="inlineStr">
+        <is>
+          <t>In the past 7 days…</t>
+        </is>
+      </c>
+      <c r="L197" t="inlineStr">
+        <is>
+          <t>...My worries overwhelmed me</t>
+        </is>
+      </c>
+      <c r="M197" t="inlineStr"/>
+    </row>
+    <row r="198">
+      <c r="A198" s="1" t="n">
+        <v>196</v>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>PROMIS 29+2/ PROPr</t>
+        </is>
+      </c>
+      <c r="C198" t="inlineStr">
+        <is>
+          <t>p3d</t>
+        </is>
+      </c>
+      <c r="D198" t="inlineStr">
+        <is>
+          <t>p3</t>
+        </is>
+      </c>
+      <c r="E198" t="inlineStr">
+        <is>
+          <t>Feeling uneasy</t>
+        </is>
+      </c>
+      <c r="F198" t="inlineStr"/>
+      <c r="G198" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="H198" t="inlineStr"/>
+      <c r="I198" t="inlineStr"/>
+      <c r="J198" t="inlineStr">
+        <is>
+          <t>['Never', 'Rarely', 'Sometimes', 'Often', 'Always']</t>
+        </is>
+      </c>
+      <c r="K198" t="inlineStr">
+        <is>
+          <t>In the past 7 days…</t>
+        </is>
+      </c>
+      <c r="L198" t="inlineStr">
+        <is>
+          <t>...I felt uneasy</t>
+        </is>
+      </c>
+      <c r="M198" t="inlineStr"/>
+    </row>
+    <row r="199">
+      <c r="A199" s="1" t="n">
+        <v>197</v>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>PROMIS 29+2/ PROPr</t>
+        </is>
+      </c>
+      <c r="C199" t="inlineStr">
+        <is>
+          <t>p4a</t>
+        </is>
+      </c>
+      <c r="D199" t="inlineStr">
+        <is>
+          <t>p4</t>
+        </is>
+      </c>
+      <c r="E199" t="inlineStr">
+        <is>
+          <t>Feeling worthless</t>
+        </is>
+      </c>
+      <c r="F199" t="inlineStr"/>
+      <c r="G199" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="H199" t="inlineStr"/>
+      <c r="I199" t="inlineStr"/>
+      <c r="J199" t="inlineStr">
+        <is>
+          <t>['Never', 'Rarely', 'Sometimes', 'Often', 'Always']</t>
+        </is>
+      </c>
+      <c r="K199" t="inlineStr">
+        <is>
+          <t>In the past 7 days…</t>
+        </is>
+      </c>
+      <c r="L199" t="inlineStr">
+        <is>
+          <t>...I felt worthless</t>
+        </is>
+      </c>
+      <c r="M199" t="inlineStr"/>
+    </row>
+    <row r="200">
+      <c r="A200" s="1" t="n">
+        <v>198</v>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>PROMIS 29+2/ PROPr</t>
+        </is>
+      </c>
+      <c r="C200" t="inlineStr">
+        <is>
+          <t>p4b</t>
+        </is>
+      </c>
+      <c r="D200" t="inlineStr">
+        <is>
+          <t>p4</t>
+        </is>
+      </c>
+      <c r="E200" t="inlineStr">
+        <is>
+          <t>Feeling helpless</t>
+        </is>
+      </c>
+      <c r="F200" t="inlineStr"/>
+      <c r="G200" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="H200" t="inlineStr"/>
+      <c r="I200" t="inlineStr"/>
+      <c r="J200" t="inlineStr">
+        <is>
+          <t>['Never', 'Rarely', 'Sometimes', 'Often', 'Always']</t>
+        </is>
+      </c>
+      <c r="K200" t="inlineStr">
+        <is>
+          <t>In the past 7 days…</t>
+        </is>
+      </c>
+      <c r="L200" t="inlineStr">
+        <is>
+          <t>...I felt helpless</t>
+        </is>
+      </c>
+      <c r="M200" t="inlineStr"/>
+    </row>
+    <row r="201">
+      <c r="A201" s="1" t="n">
+        <v>199</v>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>PROMIS 29+2/ PROPr</t>
+        </is>
+      </c>
+      <c r="C201" t="inlineStr">
+        <is>
+          <t>p4c</t>
+        </is>
+      </c>
+      <c r="D201" t="inlineStr">
+        <is>
+          <t>p4</t>
+        </is>
+      </c>
+      <c r="E201" t="inlineStr">
+        <is>
+          <t>Feeling depressed</t>
+        </is>
+      </c>
+      <c r="F201" t="inlineStr"/>
+      <c r="G201" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="H201" t="inlineStr"/>
+      <c r="I201" t="inlineStr"/>
+      <c r="J201" t="inlineStr">
+        <is>
+          <t>['Never', 'Rarely', 'Sometimes', 'Often', 'Always']</t>
+        </is>
+      </c>
+      <c r="K201" t="inlineStr">
+        <is>
+          <t>In the past 7 days…</t>
+        </is>
+      </c>
+      <c r="L201" t="inlineStr">
+        <is>
+          <t>...I felt depressed</t>
+        </is>
+      </c>
+      <c r="M201" t="inlineStr"/>
+    </row>
+    <row r="202">
+      <c r="A202" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>PROMIS 29+2/ PROPr</t>
+        </is>
+      </c>
+      <c r="C202" t="inlineStr">
+        <is>
+          <t>p4d</t>
+        </is>
+      </c>
+      <c r="D202" t="inlineStr">
+        <is>
+          <t>p4</t>
+        </is>
+      </c>
+      <c r="E202" t="inlineStr">
+        <is>
+          <t>Feeling hopeless</t>
+        </is>
+      </c>
+      <c r="F202" t="inlineStr"/>
+      <c r="G202" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="H202" t="inlineStr"/>
+      <c r="I202" t="inlineStr"/>
+      <c r="J202" t="inlineStr">
+        <is>
+          <t>['Never', 'Rarely', 'Sometimes', 'Often', 'Always']</t>
+        </is>
+      </c>
+      <c r="K202" t="inlineStr">
+        <is>
+          <t>In the past 7 days…</t>
+        </is>
+      </c>
+      <c r="L202" t="inlineStr">
+        <is>
+          <t>...I felt hopeless</t>
+        </is>
+      </c>
+      <c r="M202" t="inlineStr"/>
+    </row>
+    <row r="203">
+      <c r="A203" s="1" t="n">
+        <v>201</v>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>PROMIS 29+2/ PROPr</t>
+        </is>
+      </c>
+      <c r="C203" t="inlineStr">
+        <is>
+          <t>p5a</t>
+        </is>
+      </c>
+      <c r="D203" t="inlineStr">
+        <is>
+          <t>p5</t>
+        </is>
+      </c>
+      <c r="E203" t="inlineStr">
+        <is>
+          <t>Feeling fatigued</t>
+        </is>
+      </c>
+      <c r="F203" t="inlineStr"/>
+      <c r="G203" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="H203" t="inlineStr"/>
+      <c r="I203" t="inlineStr"/>
+      <c r="J203" t="inlineStr">
+        <is>
+          <t>['Not at all', 'A little bit', 'Somewhat', 'Quite a bit', 'Very much']</t>
+        </is>
+      </c>
+      <c r="K203" t="inlineStr">
+        <is>
+          <t>In the past 7 days…</t>
+        </is>
+      </c>
+      <c r="L203" t="inlineStr">
+        <is>
+          <t>...I felt fatigued</t>
+        </is>
+      </c>
+      <c r="M203" t="inlineStr"/>
+    </row>
+    <row r="204">
+      <c r="A204" s="1" t="n">
+        <v>202</v>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>PROMIS 29+2/ PROPr</t>
+        </is>
+      </c>
+      <c r="C204" t="inlineStr">
+        <is>
+          <t>p5b</t>
+        </is>
+      </c>
+      <c r="D204" t="inlineStr">
+        <is>
+          <t>p5</t>
+        </is>
+      </c>
+      <c r="E204" t="inlineStr">
+        <is>
+          <t>Trouble starting things because tired</t>
+        </is>
+      </c>
+      <c r="F204" t="inlineStr"/>
+      <c r="G204" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="H204" t="inlineStr"/>
+      <c r="I204" t="inlineStr"/>
+      <c r="J204" t="inlineStr">
+        <is>
+          <t>['Not at all', 'A little bit', 'Somewhat', 'Quite a bit', 'Very much']</t>
+        </is>
+      </c>
+      <c r="K204" t="inlineStr">
+        <is>
+          <t>In the past 7 days…</t>
+        </is>
+      </c>
+      <c r="L204" t="inlineStr">
+        <is>
+          <t>...I had trouble starting things because I was tired</t>
+        </is>
+      </c>
+      <c r="M204" t="inlineStr"/>
+    </row>
+    <row r="205">
+      <c r="A205" s="1" t="n">
+        <v>203</v>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>PROMIS 29+2/ PROPr</t>
+        </is>
+      </c>
+      <c r="C205" t="inlineStr">
+        <is>
+          <t>p5c</t>
+        </is>
+      </c>
+      <c r="D205" t="inlineStr">
+        <is>
+          <t>p5</t>
+        </is>
+      </c>
+      <c r="E205" t="inlineStr">
+        <is>
+          <t>Feeling run-down</t>
+        </is>
+      </c>
+      <c r="F205" t="inlineStr"/>
+      <c r="G205" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="H205" t="inlineStr"/>
+      <c r="I205" t="inlineStr"/>
+      <c r="J205" t="inlineStr">
+        <is>
+          <t>['Not at all', 'A little bit', 'Somewhat', 'Quite a bit', 'Very much']</t>
+        </is>
+      </c>
+      <c r="K205" t="inlineStr">
+        <is>
+          <t>In the past 7 days…</t>
+        </is>
+      </c>
+      <c r="L205" t="inlineStr">
+        <is>
+          <t>…how run-down did you feel on average?</t>
+        </is>
+      </c>
+      <c r="M205" t="inlineStr"/>
+    </row>
+    <row r="206">
+      <c r="A206" s="1" t="n">
+        <v>204</v>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>PROMIS 29+2/ PROPr</t>
+        </is>
+      </c>
+      <c r="C206" t="inlineStr">
+        <is>
+          <t>p5d</t>
+        </is>
+      </c>
+      <c r="D206" t="inlineStr">
+        <is>
+          <t>p5</t>
+        </is>
+      </c>
+      <c r="E206" t="inlineStr">
+        <is>
+          <t>Fatigue level</t>
+        </is>
+      </c>
+      <c r="F206" t="inlineStr"/>
+      <c r="G206" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="H206" t="inlineStr"/>
+      <c r="I206" t="inlineStr"/>
+      <c r="J206" t="inlineStr">
+        <is>
+          <t>['Not at all', 'A little bit', 'Somewhat', 'Quite a bit', 'Very much']</t>
+        </is>
+      </c>
+      <c r="K206" t="inlineStr">
+        <is>
+          <t>In the past 7 days…</t>
+        </is>
+      </c>
+      <c r="L206" t="inlineStr">
+        <is>
+          <t>…how fatigued were you on average?</t>
+        </is>
+      </c>
+      <c r="M206" t="inlineStr"/>
+    </row>
+    <row r="207">
+      <c r="A207" s="1" t="n">
+        <v>205</v>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>PROMIS 29+2/ PROPr</t>
+        </is>
+      </c>
+      <c r="C207" t="inlineStr">
+        <is>
+          <t>p6a</t>
+        </is>
+      </c>
+      <c r="D207" t="inlineStr">
+        <is>
+          <t>p6</t>
+        </is>
+      </c>
+      <c r="E207" t="inlineStr">
+        <is>
+          <t>Sleep quality</t>
+        </is>
+      </c>
+      <c r="F207" t="inlineStr"/>
+      <c r="G207" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="H207" t="inlineStr"/>
+      <c r="I207" t="inlineStr"/>
+      <c r="J207" t="inlineStr">
+        <is>
+          <t>['Very poor', 'Poor', 'Fair', 'Good', 'Very good']</t>
+        </is>
+      </c>
+      <c r="K207" t="inlineStr">
+        <is>
+          <t>In the past 7 days…</t>
+        </is>
+      </c>
+      <c r="L207" t="inlineStr">
+        <is>
+          <t>...my sleep quality was</t>
+        </is>
+      </c>
+      <c r="M207" t="inlineStr"/>
+    </row>
+    <row r="208">
+      <c r="A208" s="1" t="n">
+        <v>206</v>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>PROMIS 29+2/ PROPr</t>
+        </is>
+      </c>
+      <c r="C208" t="inlineStr">
+        <is>
+          <t>p6b</t>
+        </is>
+      </c>
+      <c r="D208" t="inlineStr">
+        <is>
+          <t>p6</t>
+        </is>
+      </c>
+      <c r="E208" t="inlineStr">
+        <is>
+          <t>Refreshing sleep</t>
+        </is>
+      </c>
+      <c r="F208" t="inlineStr"/>
+      <c r="G208" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="H208" t="inlineStr"/>
+      <c r="I208" t="inlineStr"/>
+      <c r="J208" t="inlineStr">
+        <is>
+          <t>['Not at all', 'A little bit', 'Somewhat', 'Quite a bit', 'Very much']</t>
+        </is>
+      </c>
+      <c r="K208" t="inlineStr">
+        <is>
+          <t>In the past 7 days…</t>
+        </is>
+      </c>
+      <c r="L208" t="inlineStr">
+        <is>
+          <t>...my sleep was refreshing</t>
+        </is>
+      </c>
+      <c r="M208" t="inlineStr"/>
+    </row>
+    <row r="209">
+      <c r="A209" s="1" t="n">
+        <v>207</v>
+      </c>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>PROMIS 29+2/ PROPr</t>
+        </is>
+      </c>
+      <c r="C209" t="inlineStr">
+        <is>
+          <t>p6c</t>
+        </is>
+      </c>
+      <c r="D209" t="inlineStr">
+        <is>
+          <t>p6</t>
+        </is>
+      </c>
+      <c r="E209" t="inlineStr">
+        <is>
+          <t>Sleep problems</t>
+        </is>
+      </c>
+      <c r="F209" t="inlineStr"/>
+      <c r="G209" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="H209" t="inlineStr"/>
+      <c r="I209" t="inlineStr"/>
+      <c r="J209" t="inlineStr">
+        <is>
+          <t>['Not at all', 'A little bit', 'Somewhat', 'Quite a bit', 'Very much']</t>
+        </is>
+      </c>
+      <c r="K209" t="inlineStr">
+        <is>
+          <t>In the past 7 days…</t>
+        </is>
+      </c>
+      <c r="L209" t="inlineStr">
+        <is>
+          <t>...I had problems with my sleep</t>
+        </is>
+      </c>
+      <c r="M209" t="inlineStr"/>
+    </row>
+    <row r="210">
+      <c r="A210" s="1" t="n">
+        <v>208</v>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>PROMIS 29+2/ PROPr</t>
+        </is>
+      </c>
+      <c r="C210" t="inlineStr">
+        <is>
+          <t>p6d</t>
+        </is>
+      </c>
+      <c r="D210" t="inlineStr">
+        <is>
+          <t>p6</t>
+        </is>
+      </c>
+      <c r="E210" t="inlineStr">
+        <is>
+          <t>Difficulty falling asleep</t>
+        </is>
+      </c>
+      <c r="F210" t="inlineStr"/>
+      <c r="G210" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="H210" t="inlineStr"/>
+      <c r="I210" t="inlineStr"/>
+      <c r="J210" t="inlineStr">
+        <is>
+          <t>['Not at all', 'A little bit', 'Somewhat', 'Quite a bit', 'Very much']</t>
+        </is>
+      </c>
+      <c r="K210" t="inlineStr">
+        <is>
+          <t>In the past 7 days…</t>
+        </is>
+      </c>
+      <c r="L210" t="inlineStr">
+        <is>
+          <t>...I had difficulty falling asleep</t>
+        </is>
+      </c>
+      <c r="M210" t="inlineStr"/>
+    </row>
+    <row r="211">
+      <c r="A211" s="1" t="n">
+        <v>209</v>
+      </c>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t>PROMIS 29+2/ PROPr</t>
+        </is>
+      </c>
+      <c r="C211" t="inlineStr">
+        <is>
+          <t>p7a</t>
+        </is>
+      </c>
+      <c r="D211" t="inlineStr">
+        <is>
+          <t>p7</t>
+        </is>
+      </c>
+      <c r="E211" t="inlineStr">
+        <is>
+          <t>Concentration</t>
+        </is>
+      </c>
+      <c r="F211" t="inlineStr"/>
+      <c r="G211" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="H211" t="inlineStr"/>
+      <c r="I211" t="inlineStr"/>
+      <c r="J211" t="inlineStr">
+        <is>
+          <t>['Not at all', 'A little bit', 'Somewhat', 'Quite a bit', 'Very much']</t>
+        </is>
+      </c>
+      <c r="K211" t="inlineStr">
+        <is>
+          <t>In the past 7 days…</t>
+        </is>
+      </c>
+      <c r="L211" t="inlineStr">
+        <is>
+          <t>...I have been able to concentrate</t>
+        </is>
+      </c>
+      <c r="M211" t="inlineStr"/>
+    </row>
+    <row r="212">
+      <c r="A212" s="1" t="n">
+        <v>210</v>
+      </c>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>PROMIS 29+2/ PROPr</t>
+        </is>
+      </c>
+      <c r="C212" t="inlineStr">
+        <is>
+          <t>p7b</t>
+        </is>
+      </c>
+      <c r="D212" t="inlineStr">
+        <is>
+          <t>p7</t>
+        </is>
+      </c>
+      <c r="E212" t="inlineStr">
+        <is>
+          <t>Remembering things</t>
+        </is>
+      </c>
+      <c r="F212" t="inlineStr"/>
+      <c r="G212" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="H212" t="inlineStr"/>
+      <c r="I212" t="inlineStr"/>
+      <c r="J212" t="inlineStr">
+        <is>
+          <t>['Not at all', 'A little bit', 'Somewhat', 'Quite a bit', 'Very much']</t>
+        </is>
+      </c>
+      <c r="K212" t="inlineStr">
+        <is>
+          <t>In the past 7 days…</t>
+        </is>
+      </c>
+      <c r="L212" t="inlineStr">
+        <is>
+          <t>...I have been able to remember to do things, like take medicine or buy something I needed</t>
+        </is>
+      </c>
+      <c r="M212" t="inlineStr"/>
+    </row>
+    <row r="213">
+      <c r="A213" s="1" t="n">
+        <v>211</v>
+      </c>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>PROMIS 29+2/ PROPr</t>
+        </is>
+      </c>
+      <c r="C213" t="inlineStr">
+        <is>
+          <t>p8a</t>
+        </is>
+      </c>
+      <c r="D213" t="inlineStr">
+        <is>
+          <t>p8</t>
+        </is>
+      </c>
+      <c r="E213" t="inlineStr">
+        <is>
+          <t>Pain interference with day to day activity</t>
+        </is>
+      </c>
+      <c r="F213" t="inlineStr"/>
+      <c r="G213" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="H213" t="inlineStr"/>
+      <c r="I213" t="inlineStr"/>
+      <c r="J213" t="inlineStr">
+        <is>
+          <t>['Not at all', 'A little bit', 'Somewhat', 'Quite a bit', 'Very much']</t>
+        </is>
+      </c>
+      <c r="K213" t="inlineStr">
+        <is>
+          <t>In the past 7 days…</t>
+        </is>
+      </c>
+      <c r="L213" t="inlineStr">
+        <is>
+          <t>...How much did pain interfere with your day to day activities?</t>
+        </is>
+      </c>
+      <c r="M213" t="inlineStr"/>
+    </row>
+    <row r="214">
+      <c r="A214" s="1" t="n">
+        <v>212</v>
+      </c>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t>PROMIS 29+2/ PROPr</t>
+        </is>
+      </c>
+      <c r="C214" t="inlineStr">
+        <is>
+          <t>p8b</t>
+        </is>
+      </c>
+      <c r="D214" t="inlineStr">
+        <is>
+          <t>p8</t>
+        </is>
+      </c>
+      <c r="E214" t="inlineStr">
+        <is>
+          <t>Pain inteference with home work</t>
+        </is>
+      </c>
+      <c r="F214" t="inlineStr"/>
+      <c r="G214" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="H214" t="inlineStr"/>
+      <c r="I214" t="inlineStr"/>
+      <c r="J214" t="inlineStr">
+        <is>
+          <t>['Not at all', 'A little bit', 'Somewhat', 'Quite a bit', 'Very much']</t>
+        </is>
+      </c>
+      <c r="K214" t="inlineStr">
+        <is>
+          <t>In the past 7 days…</t>
+        </is>
+      </c>
+      <c r="L214" t="inlineStr">
+        <is>
+          <t>...How much did pain interfere with work around the home?</t>
+        </is>
+      </c>
+      <c r="M214" t="inlineStr"/>
+    </row>
+    <row r="215">
+      <c r="A215" s="1" t="n">
+        <v>213</v>
+      </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t>PROMIS 29+2/ PROPr</t>
+        </is>
+      </c>
+      <c r="C215" t="inlineStr">
+        <is>
+          <t>p8c</t>
+        </is>
+      </c>
+      <c r="D215" t="inlineStr">
+        <is>
+          <t>p8</t>
+        </is>
+      </c>
+      <c r="E215" t="inlineStr">
+        <is>
+          <t>Pain interference with social activities</t>
+        </is>
+      </c>
+      <c r="F215" t="inlineStr"/>
+      <c r="G215" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="H215" t="inlineStr"/>
+      <c r="I215" t="inlineStr"/>
+      <c r="J215" t="inlineStr">
+        <is>
+          <t>['Not at all', 'A little bit', 'Somewhat', 'Quite a bit', 'Very much']</t>
+        </is>
+      </c>
+      <c r="K215" t="inlineStr">
+        <is>
+          <t>In the past 7 days…</t>
+        </is>
+      </c>
+      <c r="L215" t="inlineStr">
+        <is>
+          <t>...How much did pain interfere with your ability to participate in social activities?</t>
+        </is>
+      </c>
+      <c r="M215" t="inlineStr"/>
+    </row>
+    <row r="216">
+      <c r="A216" s="1" t="n">
+        <v>214</v>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>PROMIS 29+2/ PROPr</t>
+        </is>
+      </c>
+      <c r="C216" t="inlineStr">
+        <is>
+          <t>p8d</t>
+        </is>
+      </c>
+      <c r="D216" t="inlineStr">
+        <is>
+          <t>p8</t>
+        </is>
+      </c>
+      <c r="E216" t="inlineStr">
+        <is>
+          <t>Pain interference with household chores</t>
+        </is>
+      </c>
+      <c r="F216" t="inlineStr"/>
+      <c r="G216" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="H216" t="inlineStr"/>
+      <c r="I216" t="inlineStr"/>
+      <c r="J216" t="inlineStr">
+        <is>
+          <t>['Not at all', 'A little bit', 'Somewhat', 'Quite a bit', 'Very much']</t>
+        </is>
+      </c>
+      <c r="K216" t="inlineStr">
+        <is>
+          <t>In the past 7 days…</t>
+        </is>
+      </c>
+      <c r="L216" t="inlineStr">
+        <is>
+          <t>...How much did pain interfere with your household chores?</t>
+        </is>
+      </c>
+      <c r="M216" t="inlineStr"/>
+    </row>
+    <row r="217">
+      <c r="A217" s="1" t="n">
+        <v>215</v>
+      </c>
+      <c r="B217" t="inlineStr">
+        <is>
+          <t>PROMIS 29+2/ PROPr</t>
+        </is>
+      </c>
+      <c r="C217" t="inlineStr">
+        <is>
+          <t>p9</t>
+        </is>
+      </c>
+      <c r="D217" t="inlineStr">
+        <is>
+          <t>p9</t>
+        </is>
+      </c>
+      <c r="E217" t="inlineStr">
+        <is>
+          <t>Pain intensity rating</t>
+        </is>
+      </c>
+      <c r="F217" t="inlineStr"/>
+      <c r="G217" t="inlineStr">
+        <is>
+          <t>integer</t>
+        </is>
+      </c>
+      <c r="H217" t="inlineStr"/>
+      <c r="I217" t="inlineStr"/>
+      <c r="J217" t="inlineStr"/>
+      <c r="K217" t="inlineStr">
+        <is>
+          <t>For the next question, please responds on scale from 0 being no pain to 10 being the worst pain imaginable.</t>
+        </is>
+      </c>
+      <c r="L217" t="inlineStr">
+        <is>
+          <t>In the past 7 days, how would you rate your pain on average?</t>
+        </is>
+      </c>
+      <c r="M217" t="inlineStr"/>
+    </row>
+    <row r="218">
+      <c r="A218" s="1" t="n">
+        <v>216</v>
+      </c>
+      <c r="B218" t="inlineStr">
+        <is>
+          <t>Risk of Harms and Consequences</t>
+        </is>
+      </c>
+      <c r="C218" t="inlineStr">
+        <is>
+          <t>r1a</t>
+        </is>
+      </c>
+      <c r="D218" t="inlineStr">
+        <is>
+          <t>r1</t>
+        </is>
+      </c>
+      <c r="E218" t="inlineStr">
+        <is>
+          <t>Multiple sex partners</t>
+        </is>
+      </c>
+      <c r="F218" t="inlineStr"/>
+      <c r="G218" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="H218" t="inlineStr"/>
+      <c r="I218" t="inlineStr"/>
+      <c r="J218" t="inlineStr">
+        <is>
+          <t>['Never', 'More than a year ago', '4 to 12 months ago', '2 to 3 months ago', 'Past month', 'Do not know', 'Not reported']</t>
+        </is>
+      </c>
+      <c r="K218" t="inlineStr">
+        <is>
+          <t>When was the last time you…</t>
+        </is>
+      </c>
+      <c r="L218" t="inlineStr">
+        <is>
+          <t>…had two or more sex partners during the same time period?</t>
+        </is>
+      </c>
+      <c r="M218" t="inlineStr">
+        <is>
+          <t>RECOMMENDED:  BEFORE SENSITIVE ITEMS SUCH AS THIS REMIND RESPONDENT ABOUT CONFIDENTIALITY OF INTERVIEW AND SECURITY PROCEDURES TO PROTECT DATA AND THAT THERE ARE NO ADVERSE CONSEQUENCES FOR PARTICIPATION IN SURVEY/INTERVIEW (CONSISTENT WITH HUB CONSENT FORMS)</t>
+        </is>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" s="1" t="n">
+        <v>217</v>
+      </c>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t>Risk of Harms and Consequences</t>
+        </is>
+      </c>
+      <c r="C219" t="inlineStr">
+        <is>
+          <t>r1b</t>
+        </is>
+      </c>
+      <c r="D219" t="inlineStr">
+        <is>
+          <t>r1</t>
+        </is>
+      </c>
+      <c r="E219" t="inlineStr">
+        <is>
+          <t>Unprotected sex</t>
+        </is>
+      </c>
+      <c r="F219" t="inlineStr"/>
+      <c r="G219" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="H219" t="inlineStr"/>
+      <c r="I219" t="inlineStr"/>
+      <c r="J219" t="inlineStr">
+        <is>
+          <t>['Never', 'More than a year ago', '4 to 12 months ago', '2 to 3 months ago', 'Past month', 'Do not know', 'Not reported']</t>
+        </is>
+      </c>
+      <c r="K219" t="inlineStr">
+        <is>
+          <t>When was the last time you…</t>
+        </is>
+      </c>
+      <c r="L219" t="inlineStr">
+        <is>
+          <t>…had sex without using any kind of condom, dental dam or other barrier to protect you and your partner from diseases or pregnancy?</t>
+        </is>
+      </c>
+      <c r="M219" t="inlineStr">
+        <is>
+          <t>RECOMMENDED:  BEFORE SENSITIVE ITEMS SUCH AS THIS REMIND RESPONDENT ABOUT CONFIDENTIALITY OF INTERVIEW AND SECURITY PROCEDURES TO PROTECT DATA AND THAT THERE ARE NO ADVERSE CONSEQUENCES FOR PARTICIPATION IN SURVEY/INTERVIEW (CONSISTENT WITH HUB CONSENT FORMS)</t>
+        </is>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" s="1" t="n">
+        <v>218</v>
+      </c>
+      <c r="B220" t="inlineStr">
+        <is>
+          <t>Risk of Harms and Consequences</t>
+        </is>
+      </c>
+      <c r="C220" t="inlineStr">
+        <is>
+          <t>r1c</t>
+        </is>
+      </c>
+      <c r="D220" t="inlineStr">
+        <is>
+          <t>r1</t>
+        </is>
+      </c>
+      <c r="E220" t="inlineStr">
+        <is>
+          <t>Alcohol and drug intoxication</t>
+        </is>
+      </c>
+      <c r="F220" t="inlineStr"/>
+      <c r="G220" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="H220" t="inlineStr"/>
+      <c r="I220" t="inlineStr"/>
+      <c r="J220" t="inlineStr">
+        <is>
+          <t>['Never', 'More than a year ago', '4 to 12 months ago', '2 to 3 months ago', 'Past month', 'Do not know', 'Not reported']</t>
+        </is>
+      </c>
+      <c r="K220" t="inlineStr">
+        <is>
+          <t>When was the last time you…</t>
+        </is>
+      </c>
+      <c r="L220" t="inlineStr">
+        <is>
+          <t>…had sex while you or your partner was intoxicated from alcohol or other drugs?</t>
+        </is>
+      </c>
+      <c r="M220" t="inlineStr">
+        <is>
+          <t>RECOMMENDED:  BEFORE SENSITIVE ITEMS SUCH AS THIS REMIND RESPONDENT ABOUT CONFIDENTIALITY OF INTERVIEW AND SECURITY PROCEDURES TO PROTECT DATA AND THAT THERE ARE NO ADVERSE CONSEQUENCES FOR PARTICIPATION IN SURVEY/INTERVIEW (CONSISTENT WITH HUB CONSENT FORMS)</t>
+        </is>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" s="1" t="n">
+        <v>219</v>
+      </c>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t>Risk of Harms and Consequences</t>
+        </is>
+      </c>
+      <c r="C221" t="inlineStr">
+        <is>
+          <t>r1d</t>
+        </is>
+      </c>
+      <c r="D221" t="inlineStr">
+        <is>
+          <t>r1</t>
+        </is>
+      </c>
+      <c r="E221" t="inlineStr">
+        <is>
+          <t>Drug injection with needle</t>
+        </is>
+      </c>
+      <c r="F221" t="inlineStr"/>
+      <c r="G221" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="H221" t="inlineStr"/>
+      <c r="I221" t="inlineStr"/>
+      <c r="J221" t="inlineStr">
+        <is>
+          <t>['Never', 'More than a year ago', '4 to 12 months ago', '2 to 3 months ago', 'Past month', 'Do not know', 'Not reported']</t>
+        </is>
+      </c>
+      <c r="K221" t="inlineStr">
+        <is>
+          <t>When was the last time you…</t>
+        </is>
+      </c>
+      <c r="L221" t="inlineStr">
+        <is>
+          <t>…used a needle to inject drugs like heroin, cocaine or amphetamines?</t>
+        </is>
+      </c>
+      <c r="M221" t="inlineStr">
+        <is>
+          <t>RECOMMENDED:  BEFORE SENSITIVE ITEMS SUCH AS THIS REMIND RESPONDENT ABOUT CONFIDENTIALITY OF INTERVIEW AND SECURITY PROCEDURES TO PROTECT DATA AND THAT THERE ARE NO ADVERSE CONSEQUENCES FOR PARTICIPATION IN SURVEY/INTERVIEW (CONSISTENT WITH HUB CONSENT FORMS)</t>
+        </is>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" s="1" t="n">
+        <v>220</v>
+      </c>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t>Risk of Harms and Consequences</t>
+        </is>
+      </c>
+      <c r="C222" t="inlineStr">
+        <is>
+          <t>r1g</t>
+        </is>
+      </c>
+      <c r="D222" t="inlineStr">
+        <is>
+          <t>r1</t>
+        </is>
+      </c>
+      <c r="E222" t="inlineStr">
+        <is>
+          <t>Attacked with weapon</t>
+        </is>
+      </c>
+      <c r="F222" t="inlineStr"/>
+      <c r="G222" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="H222" t="inlineStr"/>
+      <c r="I222" t="inlineStr"/>
+      <c r="J222" t="inlineStr">
+        <is>
+          <t>['Never', 'More than a year ago', '4 to 12 months ago', '2 to 3 months ago', 'Past month', 'Do not know', 'Not reported']</t>
+        </is>
+      </c>
+      <c r="K222" t="inlineStr">
+        <is>
+          <t>When was the last time you…</t>
+        </is>
+      </c>
+      <c r="L222" t="inlineStr">
+        <is>
+          <t>…were attacked with a weapon, including a gun, knife, stick, bottle or other weapon?</t>
+        </is>
+      </c>
+      <c r="M222" t="inlineStr">
+        <is>
+          <t>RECOMMENDED:  BEFORE SENSITIVE ITEMS SUCH AS THIS REMIND RESPONDENT ABOUT CONFIDENTIALITY OF INTERVIEW AND SECURITY PROCEDURES TO PROTECT DATA AND THAT THERE ARE NO ADVERSE CONSEQUENCES FOR PARTICIPATION IN SURVEY/INTERVIEW (CONSISTENT WITH HUB CONSENT FORMS)</t>
+        </is>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" s="1" t="n">
+        <v>221</v>
+      </c>
+      <c r="B223" t="inlineStr">
+        <is>
+          <t>Risk of Harms and Consequences</t>
+        </is>
+      </c>
+      <c r="C223" t="inlineStr">
+        <is>
+          <t>r1h</t>
+        </is>
+      </c>
+      <c r="D223" t="inlineStr">
+        <is>
+          <t>r1</t>
+        </is>
+      </c>
+      <c r="E223" t="inlineStr">
+        <is>
+          <t>Physical abuse</t>
+        </is>
+      </c>
+      <c r="F223" t="inlineStr"/>
+      <c r="G223" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="H223" t="inlineStr"/>
+      <c r="I223" t="inlineStr"/>
+      <c r="J223" t="inlineStr">
+        <is>
+          <t>['Never', 'More than a year ago', '4 to 12 months ago', '2 to 3 months ago', 'Past month', 'Do not know', 'Not reported']</t>
+        </is>
+      </c>
+      <c r="K223" t="inlineStr">
+        <is>
+          <t>When was the last time you…</t>
+        </is>
+      </c>
+      <c r="L223" t="inlineStr">
+        <is>
+          <t>…were physically abused, to the point that you had bruises, cuts or broken bones?</t>
+        </is>
+      </c>
+      <c r="M223" t="inlineStr">
+        <is>
+          <t>RECOMMENDED:  BEFORE SENSITIVE ITEMS SUCH AS THIS REMIND RESPONDENT ABOUT CONFIDENTIALITY OF INTERVIEW AND SECURITY PROCEDURES TO PROTECT DATA AND THAT THERE ARE NO ADVERSE CONSEQUENCES FOR PARTICIPATION IN SURVEY/INTERVIEW (CONSISTENT WITH HUB CONSENT FORMS)</t>
+        </is>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" s="1" t="n">
+        <v>222</v>
+      </c>
+      <c r="B224" t="inlineStr">
+        <is>
+          <t>Risk of Harms and Consequences</t>
+        </is>
+      </c>
+      <c r="C224" t="inlineStr">
+        <is>
+          <t>r1j</t>
+        </is>
+      </c>
+      <c r="D224" t="inlineStr">
+        <is>
+          <t>r1</t>
+        </is>
+      </c>
+      <c r="E224" t="inlineStr">
+        <is>
+          <t>Sexually abused</t>
+        </is>
+      </c>
+      <c r="F224" t="inlineStr"/>
+      <c r="G224" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="H224" t="inlineStr"/>
+      <c r="I224" t="inlineStr"/>
+      <c r="J224" t="inlineStr">
+        <is>
+          <t>['Never', 'More than a year ago', '4 to 12 months ago', '2 to 3 months ago', 'Past month', 'Do not know', 'Not reported']</t>
+        </is>
+      </c>
+      <c r="K224" t="inlineStr">
+        <is>
+          <t>When was the last time you…</t>
+        </is>
+      </c>
+      <c r="L224" t="inlineStr">
+        <is>
+          <t>…were sexually abused, where someone pressured or forced you to participate in sexual acts against your will, including your regular sex partner, a family member or friend?</t>
+        </is>
+      </c>
+      <c r="M224" t="inlineStr">
+        <is>
+          <t>RECOMMENDED:  BEFORE SENSITIVE ITEMS SUCH AS THIS REMIND RESPONDENT ABOUT CONFIDENTIALITY OF INTERVIEW AND SECURITY PROCEDURES TO PROTECT DATA AND THAT THERE ARE NO ADVERSE CONSEQUENCES FOR PARTICIPATION IN SURVEY/INTERVIEW (CONSISTENT WITH HUB CONSENT FORMS)</t>
+        </is>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" s="1" t="n">
+        <v>223</v>
+      </c>
+      <c r="B225" t="inlineStr">
+        <is>
+          <t>Risk of Harms and Consequences</t>
+        </is>
+      </c>
+      <c r="C225" t="inlineStr">
+        <is>
+          <t>r1k</t>
+        </is>
+      </c>
+      <c r="D225" t="inlineStr">
+        <is>
+          <t>r1</t>
+        </is>
+      </c>
+      <c r="E225" t="inlineStr">
+        <is>
+          <t>Emotionally abused</t>
+        </is>
+      </c>
+      <c r="F225" t="inlineStr"/>
+      <c r="G225" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="H225" t="inlineStr"/>
+      <c r="I225" t="inlineStr"/>
+      <c r="J225" t="inlineStr">
+        <is>
+          <t>['Never', 'More than a year ago', '4 to 12 months ago', '2 to 3 months ago', 'Past month', 'Do not know', 'Not reported']</t>
+        </is>
+      </c>
+      <c r="K225" t="inlineStr">
+        <is>
+          <t>When was the last time you…</t>
+        </is>
+      </c>
+      <c r="L225" t="inlineStr">
+        <is>
+          <t>…were emotionally abused, where someone did or said things to make you feel very bad about yourself or your life?</t>
+        </is>
+      </c>
+      <c r="M225" t="inlineStr">
+        <is>
+          <t>RECOMMENDED:  BEFORE SENSITIVE ITEMS SUCH AS THIS REMIND RESPONDENT ABOUT CONFIDENTIALITY OF INTERVIEW AND SECURITY PROCEDURES TO PROTECT DATA AND THAT THERE ARE NO ADVERSE CONSEQUENCES FOR PARTICIPATION IN SURVEY/INTERVIEW (CONSISTENT WITH HUB CONSENT FORMS)</t>
+        </is>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" s="1" t="n">
+        <v>224</v>
+      </c>
+      <c r="B226" t="inlineStr">
+        <is>
+          <t>Risk of Harms and Consequences</t>
+        </is>
+      </c>
+      <c r="C226" t="inlineStr">
+        <is>
+          <t>r1m</t>
+        </is>
+      </c>
+      <c r="D226" t="inlineStr">
+        <is>
+          <t>r1</t>
+        </is>
+      </c>
+      <c r="E226" t="inlineStr">
+        <is>
+          <t>Physically, sexually, or emotionally abused</t>
+        </is>
+      </c>
+      <c r="F226" t="inlineStr"/>
+      <c r="G226" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="H226" t="inlineStr"/>
+      <c r="I226" t="inlineStr"/>
+      <c r="J226" t="inlineStr">
+        <is>
+          <t>['Never', 'More than a year ago', '4 to 12 months ago', '2 to 3 months ago', 'Past month', 'Do not know', 'Not reported']</t>
+        </is>
+      </c>
+      <c r="K226" t="inlineStr">
+        <is>
+          <t>When was the last time you…</t>
+        </is>
+      </c>
+      <c r="L226" t="inlineStr">
+        <is>
+          <t>…were physically, sexual or emotionally abused several times or over a long period of time?</t>
+        </is>
+      </c>
+      <c r="M226" t="inlineStr">
+        <is>
+          <t>RECOMMENDED:  BEFORE SENSITIVE ITEMS SUCH AS THIS REMIND RESPONDENT ABOUT CONFIDENTIALITY OF INTERVIEW AND SECURITY PROCEDURES TO PROTECT DATA AND THAT THERE ARE NO ADVERSE CONSEQUENCES FOR PARTICIPATION IN SURVEY/INTERVIEW (CONSISTENT WITH HUB CONSENT FORMS)</t>
+        </is>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" s="1" t="n">
+        <v>225</v>
+      </c>
+      <c r="B227" t="inlineStr">
+        <is>
+          <t>Risk of Harms and Consequences</t>
+        </is>
+      </c>
+      <c r="C227" t="inlineStr">
+        <is>
+          <t>r1n</t>
+        </is>
+      </c>
+      <c r="D227" t="inlineStr">
+        <is>
+          <t>r1</t>
+        </is>
+      </c>
+      <c r="E227" t="inlineStr">
+        <is>
+          <t>Afraid for life or serious injury from abuse</t>
+        </is>
+      </c>
+      <c r="F227" t="inlineStr"/>
+      <c r="G227" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="H227" t="inlineStr"/>
+      <c r="I227" t="inlineStr"/>
+      <c r="J227" t="inlineStr">
+        <is>
+          <t>['Never', 'More than a year ago', '4 to 12 months ago', '2 to 3 months ago', 'Past month', 'Do not know', 'Not reported']</t>
+        </is>
+      </c>
+      <c r="K227" t="inlineStr">
+        <is>
+          <t>When was the last time you…</t>
+        </is>
+      </c>
+      <c r="L227" t="inlineStr">
+        <is>
+          <t>…were afraid for your life or that you might be seriously injured by the abuse?</t>
+        </is>
+      </c>
+      <c r="M227" t="inlineStr">
+        <is>
+          <t>RECOMMENDED:  BEFORE SENSITIVE ITEMS SUCH AS THIS REMIND RESPONDENT ABOUT CONFIDENTIALITY OF INTERVIEW AND SECURITY PROCEDURES TO PROTECT DATA AND THAT THERE ARE NO ADVERSE CONSEQUENCES FOR PARTICIPATION IN SURVEY/INTERVIEW (CONSISTENT WITH HUB CONSENT FORMS)</t>
+        </is>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" s="1" t="n">
+        <v>226</v>
+      </c>
+      <c r="B228" t="inlineStr">
+        <is>
+          <t>Risk of Harms and Consequences</t>
+        </is>
+      </c>
+      <c r="C228" t="inlineStr">
+        <is>
+          <t>r2a</t>
+        </is>
+      </c>
+      <c r="D228" t="inlineStr">
+        <is>
+          <t>r2</t>
+        </is>
+      </c>
+      <c r="E228" t="inlineStr"/>
+      <c r="F228" t="inlineStr"/>
+      <c r="G228" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="H228" t="inlineStr"/>
+      <c r="I228" t="inlineStr"/>
+      <c r="J228" t="inlineStr">
+        <is>
+          <t>['Never', 'More than a year ago', '4 to 12 months ago', '2 to 3 months ago', 'Past month', 'Do not know', 'Not reported']</t>
+        </is>
+      </c>
+      <c r="K228" t="inlineStr">
+        <is>
+          <t>When was the last time you. . .</t>
+        </is>
+      </c>
+      <c r="L228" t="inlineStr">
+        <is>
+          <t>…became very distressed and upset when something reminded you of the past?</t>
+        </is>
+      </c>
+      <c r="M228" t="inlineStr">
+        <is>
+          <t>RECOMMENDED:  BEFORE SENSITIVE ITEMS SUCH AS THIS REMIND RESPONDENT ABOUT CONFIDENTIALITY OF INTERVIEW AND SECURITY PROCEDURES TO PROTECT DATA AND THAT THERE ARE NO ADVERSE CONSEQUENCES FOR PARTICIPATION IN SURVEY/INTERVIEW (CONSISTENT WITH HUB CONSENT FORMS)</t>
+        </is>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" s="1" t="n">
+        <v>227</v>
+      </c>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t>Risk of Harms and Consequences</t>
+        </is>
+      </c>
+      <c r="C229" t="inlineStr">
+        <is>
+          <t>r2b</t>
+        </is>
+      </c>
+      <c r="D229" t="inlineStr">
+        <is>
+          <t>r2</t>
+        </is>
+      </c>
+      <c r="E229" t="inlineStr"/>
+      <c r="F229" t="inlineStr"/>
+      <c r="G229" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="H229" t="inlineStr"/>
+      <c r="I229" t="inlineStr"/>
+      <c r="J229" t="inlineStr">
+        <is>
+          <t>['Never', 'More than a year ago', '4 to 12 months ago', '2 to 3 months ago', 'Past month', 'Do not know', 'Not reported']</t>
+        </is>
+      </c>
+      <c r="K229" t="inlineStr">
+        <is>
+          <t>When was the last time you. . .</t>
+        </is>
+      </c>
+      <c r="L229" t="inlineStr">
+        <is>
+          <t>…thought about ending your life or dying by suicide?</t>
+        </is>
+      </c>
+      <c r="M229" t="inlineStr">
+        <is>
+          <t>RECOMMENDED:  BEFORE SENSITIVE ITEMS SUCH AS THIS REMIND RESPONDENT ABOUT CONFIDENTIALITY OF INTERVIEW AND SECURITY PROCEDURES TO PROTECT DATA AND THAT THERE ARE NO ADVERSE CONSEQUENCES FOR PARTICIPATION IN SURVEY/INTERVIEW (CONSISTENT WITH HUB CONSENT FORMS)</t>
+        </is>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" s="1" t="n">
+        <v>228</v>
+      </c>
+      <c r="B230" t="inlineStr">
+        <is>
+          <t>Risk of Harms and Consequences</t>
+        </is>
+      </c>
+      <c r="C230" t="inlineStr">
+        <is>
+          <t>r3a</t>
+        </is>
+      </c>
+      <c r="D230" t="inlineStr">
+        <is>
+          <t>r3</t>
+        </is>
+      </c>
+      <c r="E230" t="inlineStr"/>
+      <c r="F230" t="inlineStr"/>
+      <c r="G230" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="H230" t="inlineStr"/>
+      <c r="I230" t="inlineStr"/>
+      <c r="J230" t="inlineStr">
+        <is>
+          <t>['Yes', 'No', "Don't recall"]</t>
+        </is>
+      </c>
+      <c r="K230" t="inlineStr">
+        <is>
+          <t>Were you ever told by a doctor or nurse that you had…</t>
+        </is>
+      </c>
+      <c r="L230" t="inlineStr">
+        <is>
+          <t>Human Immunodeficiency Virus, HIV or AIDS?</t>
+        </is>
+      </c>
+      <c r="M230" t="inlineStr">
+        <is>
+          <t>RECOMMENDED:  BEFORE SENSITIVE ITEMS SUCH AS THIS REMIND RESPONDENT ABOUT CONFIDENTIALITY OF INTERVIEW AND SECURITY PROCEDURES TO PROTECT DATA AND THAT THERE ARE NO ADVERSE CONSEQUENCES FOR PARTICIPATION IN SURVEY/INTERVIEW (CONSISTENT WITH HUB CONSENT FORMS)</t>
+        </is>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" s="1" t="n">
+        <v>229</v>
+      </c>
+      <c r="B231" t="inlineStr">
+        <is>
+          <t>Risk of Harms and Consequences</t>
+        </is>
+      </c>
+      <c r="C231" t="inlineStr">
+        <is>
+          <t>r3b</t>
+        </is>
+      </c>
+      <c r="D231" t="inlineStr">
+        <is>
+          <t>r3</t>
+        </is>
+      </c>
+      <c r="E231" t="inlineStr"/>
+      <c r="F231" t="inlineStr"/>
+      <c r="G231" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="H231" t="inlineStr"/>
+      <c r="I231" t="inlineStr"/>
+      <c r="J231" t="inlineStr">
+        <is>
+          <t>['Yes', 'No', "Don't recall"]</t>
+        </is>
+      </c>
+      <c r="K231" t="inlineStr">
+        <is>
+          <t>Were you ever told by a doctor or nurse that you had…</t>
+        </is>
+      </c>
+      <c r="L231" t="inlineStr">
+        <is>
+          <t>Hepatitis C?</t>
+        </is>
+      </c>
+      <c r="M231" t="inlineStr">
+        <is>
+          <t>RECOMMENDED:  BEFORE SENSITIVE ITEMS SUCH AS THIS REMIND RESPONDENT ABOUT CONFIDENTIALITY OF INTERVIEW AND SECURITY PROCEDURES TO PROTECT DATA AND THAT THERE ARE NO ADVERSE CONSEQUENCES FOR PARTICIPATION IN SURVEY/INTERVIEW (CONSISTENT WITH HUB CONSENT FORMS)</t>
+        </is>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" s="1" t="n">
+        <v>230</v>
+      </c>
+      <c r="B232" t="inlineStr">
+        <is>
+          <t>Risk of Harms and Consequences</t>
+        </is>
+      </c>
+      <c r="C232" t="inlineStr">
+        <is>
+          <t>r3c</t>
+        </is>
+      </c>
+      <c r="D232" t="inlineStr">
+        <is>
+          <t>r3</t>
+        </is>
+      </c>
+      <c r="E232" t="inlineStr"/>
+      <c r="F232" t="inlineStr"/>
+      <c r="G232" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="H232" t="inlineStr"/>
+      <c r="I232" t="inlineStr"/>
+      <c r="J232" t="inlineStr">
+        <is>
+          <t>['Yes', 'No', "Don't recall"]</t>
+        </is>
+      </c>
+      <c r="K232" t="inlineStr">
+        <is>
+          <t>Were you ever told by a doctor or nurse that you had…</t>
+        </is>
+      </c>
+      <c r="L232" t="inlineStr">
+        <is>
+          <t>Hepatitis B?</t>
+        </is>
+      </c>
+      <c r="M232" t="inlineStr">
+        <is>
+          <t>RECOMMENDED:  BEFORE SENSITIVE ITEMS SUCH AS THIS REMIND RESPONDENT ABOUT CONFIDENTIALITY OF INTERVIEW AND SECURITY PROCEDURES TO PROTECT DATA AND THAT THERE ARE NO ADVERSE CONSEQUENCES FOR PARTICIPATION IN SURVEY/INTERVIEW (CONSISTENT WITH HUB CONSENT FORMS)</t>
+        </is>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" s="1" t="n">
+        <v>231</v>
+      </c>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>Risk of Harms and Consequences</t>
+        </is>
+      </c>
+      <c r="C233" t="inlineStr">
+        <is>
+          <t>r3d</t>
+        </is>
+      </c>
+      <c r="D233" t="inlineStr">
+        <is>
+          <t>r3</t>
+        </is>
+      </c>
+      <c r="E233" t="inlineStr"/>
+      <c r="F233" t="inlineStr"/>
+      <c r="G233" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="H233" t="inlineStr"/>
+      <c r="I233" t="inlineStr"/>
+      <c r="J233" t="inlineStr">
+        <is>
+          <t>['Yes', 'No', "Don't recall"]</t>
+        </is>
+      </c>
+      <c r="K233" t="inlineStr">
+        <is>
+          <t>Were you ever told by a doctor or nurse that you had…</t>
+        </is>
+      </c>
+      <c r="L233" t="inlineStr">
+        <is>
+          <t>Other sexually transmitted diseases or infections, such as syphilis.</t>
+        </is>
+      </c>
+      <c r="M233" t="inlineStr">
+        <is>
+          <t>RECOMMENDED:  BEFORE SENSITIVE ITEMS SUCH AS THIS REMIND RESPONDENT ABOUT CONFIDENTIALITY OF INTERVIEW AND SECURITY PROCEDURES TO PROTECT DATA AND THAT THERE ARE NO ADVERSE CONSEQUENCES FOR PARTICIPATION IN SURVEY/INTERVIEW (CONSISTENT WITH HUB CONSENT FORMS)</t>
+        </is>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" s="1" t="n">
+        <v>232</v>
+      </c>
+      <c r="B234" t="inlineStr">
+        <is>
+          <t>Risk of Harms and Consequences</t>
+        </is>
+      </c>
+      <c r="C234" t="inlineStr">
+        <is>
+          <t>r3e</t>
+        </is>
+      </c>
+      <c r="D234" t="inlineStr">
+        <is>
+          <t>r3</t>
+        </is>
+      </c>
+      <c r="E234" t="inlineStr"/>
+      <c r="F234" t="inlineStr"/>
+      <c r="G234" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="H234" t="inlineStr"/>
+      <c r="I234" t="inlineStr"/>
+      <c r="J234" t="inlineStr">
+        <is>
+          <t>['Yes', 'No', "Don't recall"]</t>
+        </is>
+      </c>
+      <c r="K234" t="inlineStr">
+        <is>
+          <t>Were you ever told by a doctor or nurse that you had…</t>
+        </is>
+      </c>
+      <c r="L234" t="inlineStr">
+        <is>
+          <t>Tuberculosis or TB?</t>
+        </is>
+      </c>
+      <c r="M234" t="inlineStr">
+        <is>
+          <t>RECOMMENDED:  BEFORE SENSITIVE ITEMS SUCH AS THIS REMIND RESPONDENT ABOUT CONFIDENTIALITY OF INTERVIEW AND SECURITY PROCEDURES TO PROTECT DATA AND THAT THERE ARE NO ADVERSE CONSEQUENCES FOR PARTICIPATION IN SURVEY/INTERVIEW (CONSISTENT WITH HUB CONSENT FORMS)</t>
+        </is>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" s="1" t="n">
+        <v>233</v>
+      </c>
+      <c r="B235" t="inlineStr">
+        <is>
+          <t>Risk of Harms and Consequences</t>
+        </is>
+      </c>
+      <c r="C235" t="inlineStr">
+        <is>
+          <t>r3f</t>
+        </is>
+      </c>
+      <c r="D235" t="inlineStr">
+        <is>
+          <t>r3</t>
+        </is>
+      </c>
+      <c r="E235" t="inlineStr"/>
+      <c r="F235" t="inlineStr"/>
+      <c r="G235" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="H235" t="inlineStr"/>
+      <c r="I235" t="inlineStr"/>
+      <c r="J235" t="inlineStr">
+        <is>
+          <t>['Yes', 'No', "Don't recall"]</t>
+        </is>
+      </c>
+      <c r="K235" t="inlineStr">
+        <is>
+          <t>Were you ever told by a doctor or nurse that you had…</t>
+        </is>
+      </c>
+      <c r="L235" t="inlineStr">
+        <is>
+          <t>Coronavirus 19 or COVID19?</t>
+        </is>
+      </c>
+      <c r="M235" t="inlineStr">
+        <is>
+          <t>RECOMMENDED:  BEFORE SENSITIVE ITEMS SUCH AS THIS REMIND RESPONDENT ABOUT CONFIDENTIALITY OF INTERVIEW AND SECURITY PROCEDURES TO PROTECT DATA AND THAT THERE ARE NO ADVERSE CONSEQUENCES FOR PARTICIPATION IN SURVEY/INTERVIEW (CONSISTENT WITH HUB CONSENT FORMS)</t>
+        </is>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" s="1" t="n">
+        <v>234</v>
+      </c>
+      <c r="B236" t="inlineStr">
+        <is>
+          <t>Risk of Harms and Consequences</t>
+        </is>
+      </c>
+      <c r="C236" t="inlineStr">
+        <is>
+          <t>r3a_first_dx</t>
+        </is>
+      </c>
+      <c r="D236" t="inlineStr">
+        <is>
+          <t>r3</t>
+        </is>
+      </c>
+      <c r="E236" t="inlineStr"/>
+      <c r="F236" t="inlineStr"/>
+      <c r="G236" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="H236" t="inlineStr"/>
+      <c r="I236" t="inlineStr"/>
+      <c r="J236" t="inlineStr">
+        <is>
+          <t>['Never', 'More than a year ago', '4 to 12 months ago', '2 to 3 months ago', 'Past month', 'Do not know', 'Not reported']</t>
+        </is>
+      </c>
+      <c r="K236" t="inlineStr">
+        <is>
+          <t>If yes, when were you FIRST diagnosed?</t>
+        </is>
+      </c>
+      <c r="L236" t="inlineStr">
+        <is>
+          <t>Human Immunodeficiency Virus, HIV or AIDS?</t>
+        </is>
+      </c>
+      <c r="M236" t="inlineStr">
+        <is>
+          <t>RECOMMENDED:  BEFORE SENSITIVE ITEMS SUCH AS THIS REMIND RESPONDENT ABOUT CONFIDENTIALITY OF INTERVIEW AND SECURITY PROCEDURES TO PROTECT DATA AND THAT THERE ARE NO ADVERSE CONSEQUENCES FOR PARTICIPATION IN SURVEY/INTERVIEW (CONSISTENT WITH HUB CONSENT FORMS)</t>
+        </is>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" s="1" t="n">
+        <v>235</v>
+      </c>
+      <c r="B237" t="inlineStr">
+        <is>
+          <t>Risk of Harms and Consequences</t>
+        </is>
+      </c>
+      <c r="C237" t="inlineStr">
+        <is>
+          <t>r3b_first_dx</t>
+        </is>
+      </c>
+      <c r="D237" t="inlineStr">
+        <is>
+          <t>r3</t>
+        </is>
+      </c>
+      <c r="E237" t="inlineStr"/>
+      <c r="F237" t="inlineStr"/>
+      <c r="G237" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="H237" t="inlineStr"/>
+      <c r="I237" t="inlineStr"/>
+      <c r="J237" t="inlineStr">
+        <is>
+          <t>['Never', 'More than a year ago', '4 to 12 months ago', '2 to 3 months ago', 'Past month', 'Do not know', 'Not reported']</t>
+        </is>
+      </c>
+      <c r="K237" t="inlineStr">
+        <is>
+          <t>If yes, when were you FIRST diagnosed?</t>
+        </is>
+      </c>
+      <c r="L237" t="inlineStr">
+        <is>
+          <t>Hepatitis C?</t>
+        </is>
+      </c>
+      <c r="M237" t="inlineStr">
+        <is>
+          <t>RECOMMENDED:  BEFORE SENSITIVE ITEMS SUCH AS THIS REMIND RESPONDENT ABOUT CONFIDENTIALITY OF INTERVIEW AND SECURITY PROCEDURES TO PROTECT DATA AND THAT THERE ARE NO ADVERSE CONSEQUENCES FOR PARTICIPATION IN SURVEY/INTERVIEW (CONSISTENT WITH HUB CONSENT FORMS)</t>
+        </is>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" s="1" t="n">
+        <v>236</v>
+      </c>
+      <c r="B238" t="inlineStr">
+        <is>
+          <t>Risk of Harms and Consequences</t>
+        </is>
+      </c>
+      <c r="C238" t="inlineStr">
+        <is>
+          <t>r3c_first_dx</t>
+        </is>
+      </c>
+      <c r="D238" t="inlineStr">
+        <is>
+          <t>r3</t>
+        </is>
+      </c>
+      <c r="E238" t="inlineStr"/>
+      <c r="F238" t="inlineStr"/>
+      <c r="G238" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="H238" t="inlineStr"/>
+      <c r="I238" t="inlineStr"/>
+      <c r="J238" t="inlineStr">
+        <is>
+          <t>['Never', 'More than a year ago', '4 to 12 months ago', '2 to 3 months ago', 'Past month', 'Do not know', 'Not reported']</t>
+        </is>
+      </c>
+      <c r="K238" t="inlineStr">
+        <is>
+          <t>If yes, when were you FIRST diagnosed?</t>
+        </is>
+      </c>
+      <c r="L238" t="inlineStr">
+        <is>
+          <t>Hepatitis B?</t>
+        </is>
+      </c>
+      <c r="M238" t="inlineStr">
+        <is>
+          <t>RECOMMENDED:  BEFORE SENSITIVE ITEMS SUCH AS THIS REMIND RESPONDENT ABOUT CONFIDENTIALITY OF INTERVIEW AND SECURITY PROCEDURES TO PROTECT DATA AND THAT THERE ARE NO ADVERSE CONSEQUENCES FOR PARTICIPATION IN SURVEY/INTERVIEW (CONSISTENT WITH HUB CONSENT FORMS)</t>
+        </is>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" s="1" t="n">
+        <v>237</v>
+      </c>
+      <c r="B239" t="inlineStr">
+        <is>
+          <t>Risk of Harms and Consequences</t>
+        </is>
+      </c>
+      <c r="C239" t="inlineStr">
+        <is>
+          <t>r3d_first_dx</t>
+        </is>
+      </c>
+      <c r="D239" t="inlineStr">
+        <is>
+          <t>r3</t>
+        </is>
+      </c>
+      <c r="E239" t="inlineStr"/>
+      <c r="F239" t="inlineStr"/>
+      <c r="G239" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="H239" t="inlineStr"/>
+      <c r="I239" t="inlineStr"/>
+      <c r="J239" t="inlineStr">
+        <is>
+          <t>['Never', 'More than a year ago', '4 to 12 months ago', '2 to 3 months ago', 'Past month', 'Do not know', 'Not reported']</t>
+        </is>
+      </c>
+      <c r="K239" t="inlineStr">
+        <is>
+          <t>If yes, when were you FIRST diagnosed?</t>
+        </is>
+      </c>
+      <c r="L239" t="inlineStr">
+        <is>
+          <t>Other sexually transmitted diseases or infections, such as syphilis.</t>
+        </is>
+      </c>
+      <c r="M239" t="inlineStr">
+        <is>
+          <t>RECOMMENDED:  BEFORE SENSITIVE ITEMS SUCH AS THIS REMIND RESPONDENT ABOUT CONFIDENTIALITY OF INTERVIEW AND SECURITY PROCEDURES TO PROTECT DATA AND THAT THERE ARE NO ADVERSE CONSEQUENCES FOR PARTICIPATION IN SURVEY/INTERVIEW (CONSISTENT WITH HUB CONSENT FORMS)</t>
+        </is>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" s="1" t="n">
+        <v>238</v>
+      </c>
+      <c r="B240" t="inlineStr">
+        <is>
+          <t>Risk of Harms and Consequences</t>
+        </is>
+      </c>
+      <c r="C240" t="inlineStr">
+        <is>
+          <t>r3e_first_dx</t>
+        </is>
+      </c>
+      <c r="D240" t="inlineStr">
+        <is>
+          <t>r3</t>
+        </is>
+      </c>
+      <c r="E240" t="inlineStr"/>
+      <c r="F240" t="inlineStr"/>
+      <c r="G240" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="H240" t="inlineStr"/>
+      <c r="I240" t="inlineStr"/>
+      <c r="J240" t="inlineStr">
+        <is>
+          <t>['Never', 'More than a year ago', '4 to 12 months ago', '2 to 3 months ago', 'Past month', 'Do not know', 'Not reported']</t>
+        </is>
+      </c>
+      <c r="K240" t="inlineStr">
+        <is>
+          <t>If yes, when were you FIRST diagnosed?</t>
+        </is>
+      </c>
+      <c r="L240" t="inlineStr">
+        <is>
+          <t>Tuberculosis or TB?</t>
+        </is>
+      </c>
+      <c r="M240" t="inlineStr">
+        <is>
+          <t>RECOMMENDED:  BEFORE SENSITIVE ITEMS SUCH AS THIS REMIND RESPONDENT ABOUT CONFIDENTIALITY OF INTERVIEW AND SECURITY PROCEDURES TO PROTECT DATA AND THAT THERE ARE NO ADVERSE CONSEQUENCES FOR PARTICIPATION IN SURVEY/INTERVIEW (CONSISTENT WITH HUB CONSENT FORMS)</t>
+        </is>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" s="1" t="n">
+        <v>239</v>
+      </c>
+      <c r="B241" t="inlineStr">
+        <is>
+          <t>Risk of Harms and Consequences</t>
+        </is>
+      </c>
+      <c r="C241" t="inlineStr">
+        <is>
+          <t>r3f_first_dx</t>
+        </is>
+      </c>
+      <c r="D241" t="inlineStr">
+        <is>
+          <t>r3</t>
+        </is>
+      </c>
+      <c r="E241" t="inlineStr"/>
+      <c r="F241" t="inlineStr"/>
+      <c r="G241" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="H241" t="inlineStr"/>
+      <c r="I241" t="inlineStr"/>
+      <c r="J241" t="inlineStr">
+        <is>
+          <t>['Never', 'More than a year ago', '4 to 12 months ago', '2 to 3 months ago', 'Past month', 'Do not know', 'Not reported']</t>
+        </is>
+      </c>
+      <c r="K241" t="inlineStr">
+        <is>
+          <t>If yes, when were you FIRST diagnosed?</t>
+        </is>
+      </c>
+      <c r="L241" t="inlineStr">
+        <is>
+          <t>Coronavirus 19 or COVID19?</t>
+        </is>
+      </c>
+      <c r="M241" t="inlineStr">
+        <is>
+          <t>RECOMMENDED:  BEFORE SENSITIVE ITEMS SUCH AS THIS REMIND RESPONDENT ABOUT CONFIDENTIALITY OF INTERVIEW AND SECURITY PROCEDURES TO PROTECT DATA AND THAT THERE ARE NO ADVERSE CONSEQUENCES FOR PARTICIPATION IN SURVEY/INTERVIEW (CONSISTENT WITH HUB CONSENT FORMS)</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>